<commit_message>
Standardised file names and added filter by team name
</commit_message>
<xml_diff>
--- a/PlannerTasks.xlsx
+++ b/PlannerTasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/00c18fdba008d584/Customers (not shared)/Applepark/Power BI/Planner/PlannerWithFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F20900D7-23EB-4529-9A73-08F78B47F724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCE8DC39-43BC-44C7-99F8-6B3170D0CA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>Lists plan names</t>
   </si>
@@ -45,6 +46,9 @@
   </si>
   <si>
     <t>Plan Name</t>
+  </si>
+  <si>
+    <t>Team Name</t>
   </si>
   <si>
     <t>Lists buckets for each plan</t>
@@ -265,15 +269,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="72">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1649,6 +1655,9 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -1692,11 +1701,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0086D036-F256-4C9D-B2A1-B21C088B14C5}" name="Plan_tbl" displayName="Plan_tbl" ref="C4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
-  <autoFilter ref="C4:D5" xr:uid="{0086D036-F256-4C9D-B2A1-B21C088B14C5}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DC1DDFC2-6F8E-4F3F-AE51-F63302EFC0AE}" name="Plan ID" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{E2F1B8EB-A260-4061-B1DA-A1D4C9E02B24}" name="Plan Name" dataDxfId="67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0086D036-F256-4C9D-B2A1-B21C088B14C5}" name="Plan_tbl" displayName="Plan_tbl" ref="C4:E5" insertRow="1" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+  <autoFilter ref="C4:E5" xr:uid="{0086D036-F256-4C9D-B2A1-B21C088B14C5}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DC1DDFC2-6F8E-4F3F-AE51-F63302EFC0AE}" name="Plan ID" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{E2F1B8EB-A260-4061-B1DA-A1D4C9E02B24}" name="Plan Name" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{03F94C97-CE80-488C-BE65-16C507A1764D}" name="Team Name" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2104,35 +2114,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA97DDB5-27E3-41F9-B292-6015C745C1B8}">
-  <dimension ref="C2:D5"/>
+  <dimension ref="C2:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2147,7 +2161,7 @@
   <dimension ref="C2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2160,18 +2174,18 @@
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
@@ -2234,10 +2248,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBEBD98-CDDF-46A5-BB8F-EECC25228C81}">
-  <dimension ref="C2:AU4"/>
+  <dimension ref="C2:AU5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AU37" sqref="C5:AU37"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2280,145 +2294,192 @@
   <sheetData>
     <row r="2" spans="3:47" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="3:47" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="U4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="V4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="W4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="X4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Y4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Z4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AA4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AD4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AE4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AF4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AG4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AI4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AJ4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AK4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AL4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AM4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AN4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AO4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AP4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AQ4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AR4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AS4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AT4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AU4" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="3:47" x14ac:dyDescent="0.3">
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AP5" s="3"/>
+      <c r="AQ5" s="3"/>
+      <c r="AR5" s="3"/>
+      <c r="AS5" s="3"/>
+      <c r="AT5" s="3"/>
+      <c r="AU5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2433,7 +2494,7 @@
   <dimension ref="C2:E5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2446,7 +2507,7 @@
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
@@ -2454,10 +2515,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
@@ -2478,7 +2539,7 @@
   <dimension ref="C2:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2491,24 +2552,24 @@
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.3">
@@ -2531,7 +2592,7 @@
   <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2545,21 +2606,21 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -2574,18 +2635,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2721,18 +2782,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8039B5D0-6D3B-4FB4-B652-0338149FBDAC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E190EAA-270A-42C8-838D-8A23D09DF6DB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E190EAA-270A-42C8-838D-8A23D09DF6DB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8039B5D0-6D3B-4FB4-B652-0338149FBDAC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated to use Office Scripts to remove rows from tables
Modified the Flow to use an Office Scripts to remove all the data from the tables, prior to populating them again.  This ensures the flow runs faster and provides stability.
</commit_message>
<xml_diff>
--- a/PlannerTasks.xlsx
+++ b/PlannerTasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/00c18fdba008d584/Customers (not shared)/Applepark/Power BI/Planner/PlannerWithFlow/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCE8DC39-43BC-44C7-99F8-6B3170D0CA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD3E03FF-A982-4771-9376-7119FA789572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9468" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plans" sheetId="5" r:id="rId1"/>
@@ -269,12 +269,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2116,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA97DDB5-27E3-41F9-B292-6015C745C1B8}">
   <dimension ref="C2:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2161,7 +2159,7 @@
   <dimension ref="C2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2248,10 +2246,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBEBD98-CDDF-46A5-BB8F-EECC25228C81}">
-  <dimension ref="C2:AU5"/>
+  <dimension ref="C2:AU4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2434,53 +2432,6 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="3:47" x14ac:dyDescent="0.3">
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="3"/>
-      <c r="AJ5" s="3"/>
-      <c r="AK5" s="3"/>
-      <c r="AL5" s="3"/>
-      <c r="AM5" s="3"/>
-      <c r="AN5" s="3"/>
-      <c r="AO5" s="3"/>
-      <c r="AP5" s="3"/>
-      <c r="AQ5" s="3"/>
-      <c r="AR5" s="3"/>
-      <c r="AS5" s="3"/>
-      <c r="AT5" s="3"/>
-      <c r="AU5" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2493,8 +2444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4FB5A0-8A8A-45ED-8601-84875CAA8B86}">
   <dimension ref="C2:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2539,7 +2490,7 @@
   <dimension ref="C2:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2591,8 +2542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353B38D8-CA51-4B54-B8E6-4750BDE5CEE1}">
   <dimension ref="B2:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2641,15 +2592,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010025BF94C250D4F3428D6504CA93470C05" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0b958e8da78ae46a2ec6ca96c45141b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="05f9c4cf-3b22-4642-8b3f-b46f9e00fcab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b67ef449dd8e11e8882ef8210e0286c" ns2:_="">
     <xsd:import namespace="05f9c4cf-3b22-4642-8b3f-b46f9e00fcab"/>
@@ -2781,24 +2723,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E190EAA-270A-42C8-838D-8A23D09DF6DB}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="05f9c4cf-3b22-4642-8b3f-b46f9e00fcab"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8039B5D0-6D3B-4FB4-B652-0338149FBDAC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1F530B1-F3B4-4D56-BB52-37C0F4213D70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2814,4 +2764,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8039B5D0-6D3B-4FB4-B652-0338149FBDAC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Title column changed to text
</commit_message>
<xml_diff>
--- a/PlannerTasks.xlsx
+++ b/PlannerTasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Downloads\Planner-PowerBI-with-PowerAutomate-main\Planner-PowerBI-with-PowerAutomate-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A868E09-F295-4C7F-AD65-02FD85278A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9E26A3-C7EF-43B5-A0F5-C4B19B8CB2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9468" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plans" sheetId="5" r:id="rId1"/>
@@ -235,7 +235,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +279,87 @@
   </cellStyles>
   <dxfs count="72">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -1454,87 +1535,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1727,76 +1727,76 @@
   <autoFilter ref="C4:AU5" xr:uid="{3B8FAFF0-5141-46CD-87EE-EA0FD8F708B4}"/>
   <tableColumns count="45">
     <tableColumn id="1" xr3:uid="{2E459D10-625B-479F-964E-CB18910F1C5B}" name="Created By User Display Name" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{19E3C2A4-3DE3-4A57-B57F-76B5158D003B}" name="Created By User ID" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{C61E81F3-4EE0-49BB-876D-5EBC59B7C14E}" name="Title" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{2EA606A4-DC3C-403A-8142-44278ADC2FA2}" name="Start Date Time" dataDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{7F24A2FD-B614-4A10-9E8D-04F46B7B9657}" name="Created Date Time" dataDxfId="55"/>
-    <tableColumn id="6" xr3:uid="{0F0F9C50-58D6-4516-BD68-D67DF972F796}" name="Due Date Time" dataDxfId="54"/>
-    <tableColumn id="7" xr3:uid="{B41A123B-E630-42EF-98C4-80C71CF60B6D}" name="Completed Date Time" dataDxfId="53"/>
-    <tableColumn id="8" xr3:uid="{3C291AF8-417E-4A59-84DB-E1D5CA5A56D7}" name="Assigned To User Id" dataDxfId="52"/>
-    <tableColumn id="9" xr3:uid="{E0B0DAB3-B8FF-48B5-BFDB-307801E32EBD}" name="Assigned To User Name" dataDxfId="51"/>
-    <tableColumn id="10" xr3:uid="{C21696FF-CB83-433A-BEFC-27B3A4660644}" name="Assigned By User Id" dataDxfId="50"/>
-    <tableColumn id="11" xr3:uid="{3F540AA4-DE5A-45BF-9738-ADF98DA6D849}" name="Assigned By User Name" dataDxfId="49"/>
-    <tableColumn id="12" xr3:uid="{BAF7F7D6-EAA9-4CB9-8FB4-F18C6C3428D4}" name="Assigned Date Time" dataDxfId="48"/>
-    <tableColumn id="13" xr3:uid="{E01238AC-28AE-4663-9298-59297CAC374C}" name="Order Hint" dataDxfId="47"/>
-    <tableColumn id="14" xr3:uid="{0084CE79-479D-45ED-BB5B-118B7E8C30E1}" name="Plan Id" dataDxfId="46"/>
-    <tableColumn id="15" xr3:uid="{B814B7EB-AFA9-4858-ACC5-B2BDB7741C34}" name="Bucket Id" dataDxfId="45"/>
-    <tableColumn id="16" xr3:uid="{7E6E90BE-7BB9-408F-BACD-16130C28F4DB}" name="Bucket Name" dataDxfId="44"/>
-    <tableColumn id="17" xr3:uid="{3E0B33D4-61E0-4809-ACAB-DF32CF5BCB5D}" name="Percent Complete" dataDxfId="43"/>
-    <tableColumn id="18" xr3:uid="{AD5581C5-B64B-4542-AA4A-240691949540}" name="Reference Count" dataDxfId="42"/>
-    <tableColumn id="19" xr3:uid="{8156E264-14BA-4AC7-B844-A088235DA871}" name="Has Description" dataDxfId="41"/>
-    <tableColumn id="20" xr3:uid="{C48C896F-A466-46DE-A056-E53DE3145B7A}" name="Pink" dataDxfId="40"/>
-    <tableColumn id="21" xr3:uid="{E04DDFCE-339A-4E7B-8055-C5DAEE2A4549}" name="Red" dataDxfId="39"/>
-    <tableColumn id="22" xr3:uid="{CA1A01B6-46D8-45BE-B4CE-F8CD2C01B9AD}" name="Yellow" dataDxfId="38"/>
-    <tableColumn id="23" xr3:uid="{9AAE0049-870F-4F49-98EA-C2C9170EA2C4}" name="Green" dataDxfId="37"/>
-    <tableColumn id="24" xr3:uid="{6E09281F-6B11-435F-BE12-731F448DBE03}" name="Blue" dataDxfId="36"/>
-    <tableColumn id="25" xr3:uid="{E06796FB-1CC3-4440-8584-F2E0BE4AD908}" name="Purple" dataDxfId="35"/>
-    <tableColumn id="26" xr3:uid="{936C2ACF-8EBE-42EB-BEFC-614115AAD681}" name="Bronze" dataDxfId="34"/>
-    <tableColumn id="27" xr3:uid="{49EC973B-D185-4996-AF72-B9F677434E20}" name="Lime" dataDxfId="33"/>
-    <tableColumn id="28" xr3:uid="{F07571BD-15CB-4066-A500-50F2825A1737}" name="Aqua" dataDxfId="32"/>
-    <tableColumn id="29" xr3:uid="{B02EB03A-390A-4D71-A2F2-414515BA803E}" name="Gray" dataDxfId="31"/>
-    <tableColumn id="30" xr3:uid="{E2B4E206-0393-480B-8EBE-24031F82F509}" name="Silver" dataDxfId="30"/>
-    <tableColumn id="31" xr3:uid="{CCF19BB1-97D5-45CD-B088-AE74B8306D82}" name="Brown" dataDxfId="29"/>
-    <tableColumn id="32" xr3:uid="{E7FBBE36-3C9A-4652-BA47-F20033435ED7}" name="Cranberry" dataDxfId="28"/>
-    <tableColumn id="33" xr3:uid="{CB771C00-0A1D-40BA-8D5C-0E521CED7B3F}" name="Orange" dataDxfId="27"/>
-    <tableColumn id="34" xr3:uid="{4C415EA4-21D5-4B14-A9F7-BA7E8A94D354}" name="Peach" dataDxfId="26"/>
-    <tableColumn id="35" xr3:uid="{D1675B1C-927F-4144-9C1B-ADC4510F9986}" name="Marigold" dataDxfId="25"/>
-    <tableColumn id="36" xr3:uid="{8F80A39C-3792-457A-8DFE-14BC72A837E3}" name="Light green" dataDxfId="24"/>
-    <tableColumn id="37" xr3:uid="{4CB7B1B0-F5BE-4982-912F-1E06B9C61B29}" name="Dark green" dataDxfId="23"/>
-    <tableColumn id="38" xr3:uid="{F3C8412B-E870-47ED-9DBE-6610A8D9B783}" name="Teal" dataDxfId="22"/>
-    <tableColumn id="39" xr3:uid="{0F75FB26-236C-44D4-ACE0-EF6AA680C953}" name="Light blue" dataDxfId="21"/>
-    <tableColumn id="40" xr3:uid="{6117C392-8853-447C-8426-C1DC4CBBAC61}" name="Dark blue" dataDxfId="20"/>
-    <tableColumn id="41" xr3:uid="{CB58BF13-E845-4AAA-B5AF-52E4365071B9}" name="Lavender" dataDxfId="19"/>
-    <tableColumn id="42" xr3:uid="{37317792-D085-421D-B327-101FB71568C4}" name="Plum" dataDxfId="18"/>
-    <tableColumn id="43" xr3:uid="{4356B6CC-0814-4FF9-8BCD-0B2E8BD2EA5F}" name="Light gray" dataDxfId="17"/>
-    <tableColumn id="44" xr3:uid="{BC284A71-1A48-4C82-AF44-EF4B85E11A65}" name="Dark gray" dataDxfId="16"/>
-    <tableColumn id="45" xr3:uid="{04C79E8C-8306-4860-807D-EA3FC5968ABA}" name="Task ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{19E3C2A4-3DE3-4A57-B57F-76B5158D003B}" name="Created By User ID" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C61E81F3-4EE0-49BB-876D-5EBC59B7C14E}" name="Title" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{2EA606A4-DC3C-403A-8142-44278ADC2FA2}" name="Start Date Time" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{7F24A2FD-B614-4A10-9E8D-04F46B7B9657}" name="Created Date Time" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{0F0F9C50-58D6-4516-BD68-D67DF972F796}" name="Due Date Time" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{B41A123B-E630-42EF-98C4-80C71CF60B6D}" name="Completed Date Time" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{3C291AF8-417E-4A59-84DB-E1D5CA5A56D7}" name="Assigned To User Id" dataDxfId="55"/>
+    <tableColumn id="9" xr3:uid="{E0B0DAB3-B8FF-48B5-BFDB-307801E32EBD}" name="Assigned To User Name" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{C21696FF-CB83-433A-BEFC-27B3A4660644}" name="Assigned By User Id" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{3F540AA4-DE5A-45BF-9738-ADF98DA6D849}" name="Assigned By User Name" dataDxfId="52"/>
+    <tableColumn id="12" xr3:uid="{BAF7F7D6-EAA9-4CB9-8FB4-F18C6C3428D4}" name="Assigned Date Time" dataDxfId="51"/>
+    <tableColumn id="13" xr3:uid="{E01238AC-28AE-4663-9298-59297CAC374C}" name="Order Hint" dataDxfId="50"/>
+    <tableColumn id="14" xr3:uid="{0084CE79-479D-45ED-BB5B-118B7E8C30E1}" name="Plan Id" dataDxfId="49"/>
+    <tableColumn id="15" xr3:uid="{B814B7EB-AFA9-4858-ACC5-B2BDB7741C34}" name="Bucket Id" dataDxfId="48"/>
+    <tableColumn id="16" xr3:uid="{7E6E90BE-7BB9-408F-BACD-16130C28F4DB}" name="Bucket Name" dataDxfId="47"/>
+    <tableColumn id="17" xr3:uid="{3E0B33D4-61E0-4809-ACAB-DF32CF5BCB5D}" name="Percent Complete" dataDxfId="46"/>
+    <tableColumn id="18" xr3:uid="{AD5581C5-B64B-4542-AA4A-240691949540}" name="Reference Count" dataDxfId="45"/>
+    <tableColumn id="19" xr3:uid="{8156E264-14BA-4AC7-B844-A088235DA871}" name="Has Description" dataDxfId="44"/>
+    <tableColumn id="20" xr3:uid="{C48C896F-A466-46DE-A056-E53DE3145B7A}" name="Pink" dataDxfId="43"/>
+    <tableColumn id="21" xr3:uid="{E04DDFCE-339A-4E7B-8055-C5DAEE2A4549}" name="Red" dataDxfId="42"/>
+    <tableColumn id="22" xr3:uid="{CA1A01B6-46D8-45BE-B4CE-F8CD2C01B9AD}" name="Yellow" dataDxfId="41"/>
+    <tableColumn id="23" xr3:uid="{9AAE0049-870F-4F49-98EA-C2C9170EA2C4}" name="Green" dataDxfId="40"/>
+    <tableColumn id="24" xr3:uid="{6E09281F-6B11-435F-BE12-731F448DBE03}" name="Blue" dataDxfId="39"/>
+    <tableColumn id="25" xr3:uid="{E06796FB-1CC3-4440-8584-F2E0BE4AD908}" name="Purple" dataDxfId="38"/>
+    <tableColumn id="26" xr3:uid="{936C2ACF-8EBE-42EB-BEFC-614115AAD681}" name="Bronze" dataDxfId="37"/>
+    <tableColumn id="27" xr3:uid="{49EC973B-D185-4996-AF72-B9F677434E20}" name="Lime" dataDxfId="36"/>
+    <tableColumn id="28" xr3:uid="{F07571BD-15CB-4066-A500-50F2825A1737}" name="Aqua" dataDxfId="35"/>
+    <tableColumn id="29" xr3:uid="{B02EB03A-390A-4D71-A2F2-414515BA803E}" name="Gray" dataDxfId="34"/>
+    <tableColumn id="30" xr3:uid="{E2B4E206-0393-480B-8EBE-24031F82F509}" name="Silver" dataDxfId="33"/>
+    <tableColumn id="31" xr3:uid="{CCF19BB1-97D5-45CD-B088-AE74B8306D82}" name="Brown" dataDxfId="32"/>
+    <tableColumn id="32" xr3:uid="{E7FBBE36-3C9A-4652-BA47-F20033435ED7}" name="Cranberry" dataDxfId="31"/>
+    <tableColumn id="33" xr3:uid="{CB771C00-0A1D-40BA-8D5C-0E521CED7B3F}" name="Orange" dataDxfId="30"/>
+    <tableColumn id="34" xr3:uid="{4C415EA4-21D5-4B14-A9F7-BA7E8A94D354}" name="Peach" dataDxfId="29"/>
+    <tableColumn id="35" xr3:uid="{D1675B1C-927F-4144-9C1B-ADC4510F9986}" name="Marigold" dataDxfId="28"/>
+    <tableColumn id="36" xr3:uid="{8F80A39C-3792-457A-8DFE-14BC72A837E3}" name="Light green" dataDxfId="27"/>
+    <tableColumn id="37" xr3:uid="{4CB7B1B0-F5BE-4982-912F-1E06B9C61B29}" name="Dark green" dataDxfId="26"/>
+    <tableColumn id="38" xr3:uid="{F3C8412B-E870-47ED-9DBE-6610A8D9B783}" name="Teal" dataDxfId="25"/>
+    <tableColumn id="39" xr3:uid="{0F75FB26-236C-44D4-ACE0-EF6AA680C953}" name="Light blue" dataDxfId="24"/>
+    <tableColumn id="40" xr3:uid="{6117C392-8853-447C-8426-C1DC4CBBAC61}" name="Dark blue" dataDxfId="23"/>
+    <tableColumn id="41" xr3:uid="{CB58BF13-E845-4AAA-B5AF-52E4365071B9}" name="Lavender" dataDxfId="22"/>
+    <tableColumn id="42" xr3:uid="{37317792-D085-421D-B327-101FB71568C4}" name="Plum" dataDxfId="21"/>
+    <tableColumn id="43" xr3:uid="{4356B6CC-0814-4FF9-8BCD-0B2E8BD2EA5F}" name="Light gray" dataDxfId="20"/>
+    <tableColumn id="44" xr3:uid="{BC284A71-1A48-4C82-AF44-EF4B85E11A65}" name="Dark gray" dataDxfId="19"/>
+    <tableColumn id="45" xr3:uid="{04C79E8C-8306-4860-807D-EA3FC5968ABA}" name="Task ID" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B0BB0DD4-7A9B-4AE1-BE3C-7829BBAB7700}" name="Assignments_tbl" displayName="Assignments_tbl" ref="C4:E5" insertRow="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B0BB0DD4-7A9B-4AE1-BE3C-7829BBAB7700}" name="Assignments_tbl" displayName="Assignments_tbl" ref="C4:E5" insertRow="1" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="C4:E5" xr:uid="{6765AC4E-906D-4025-9CB2-9ADDAF4C4370}"/>
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{25BA9D37-501E-4F02-8602-955918BEA87A}" name="Plan ID" dataDxfId="12"/>
-    <tableColumn id="1" xr3:uid="{9526C529-5F41-4654-978E-F0CF011C4979}" name="Task ID" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{31883661-6848-498C-8BFC-956FCB7706FD}" name="UserAssignmentID" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{25BA9D37-501E-4F02-8602-955918BEA87A}" name="Plan ID" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{9526C529-5F41-4654-978E-F0CF011C4979}" name="Task ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{31883661-6848-498C-8BFC-956FCB7706FD}" name="UserAssignmentID" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C82BA1FC-45F4-46FA-B8A9-BF26EFB3F239}" name="User_tbl" displayName="User_tbl" ref="C4:G5" insertRow="1" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C82BA1FC-45F4-46FA-B8A9-BF26EFB3F239}" name="User_tbl" displayName="User_tbl" ref="C4:G5" insertRow="1" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="C4:G5" xr:uid="{C82BA1FC-45F4-46FA-B8A9-BF26EFB3F239}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FA0A3F04-C404-4753-A359-96D1AC675CAB}" name="Group ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{D093ED44-E1C4-4F9A-B931-0F1BCB8C046E}" name="User ID" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{941BA755-58A4-47C2-AA69-566F3CA1AEA7}" name="User Name" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{113CA927-D70C-4BBB-B346-487626583891}" name="User first name" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{9E9ED933-0DE8-4B02-89DD-490D52C7C9DE}" name="user surname" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{FA0A3F04-C404-4753-A359-96D1AC675CAB}" name="Group ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{D093ED44-E1C4-4F9A-B931-0F1BCB8C046E}" name="User ID" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{941BA755-58A4-47C2-AA69-566F3CA1AEA7}" name="User Name" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{113CA927-D70C-4BBB-B346-487626583891}" name="User first name" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{9E9ED933-0DE8-4B02-89DD-490D52C7C9DE}" name="user surname" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1806,9 +1806,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01ABAAFF-B3E2-4F16-966D-90575F6EA5BF}" name="Checklist_tbl" displayName="Checklist_tbl" ref="B4:E5" insertRow="1" totalsRowShown="0">
   <autoFilter ref="B4:E5" xr:uid="{01ABAAFF-B3E2-4F16-966D-90575F6EA5BF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D386C20E-4D87-4122-B186-7D310159AB4F}" name="TaskID" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{8A34804A-FFD7-4B4F-B4F0-B8FAD8F28324}" name="ChecklistID" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{3CC38ABB-C04A-4970-8D95-509B54B0A76E}" name="Checklist title" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D386C20E-4D87-4122-B186-7D310159AB4F}" name="TaskID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8A34804A-FFD7-4B4F-B4F0-B8FAD8F28324}" name="ChecklistID" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{3CC38ABB-C04A-4970-8D95-509B54B0A76E}" name="Checklist title" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{F00AE63D-BA73-4B1B-9D48-425CD42BE2AA}" name="Checklist is checked"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2118,19 +2118,19 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:5">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:5">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2162,20 +2162,20 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
     <col min="3" max="3" width="34" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:5">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
@@ -2186,52 +2186,52 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:5">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="3:5">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
     </row>
-    <row r="7" spans="3:5">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
     </row>
-    <row r="8" spans="3:5">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
     </row>
-    <row r="9" spans="3:5">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
     </row>
-    <row r="10" spans="3:5">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
     </row>
-    <row r="11" spans="3:5">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11"/>
     </row>
-    <row r="12" spans="3:5">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12"/>
       <c r="D12"/>
       <c r="E12"/>
     </row>
-    <row r="13" spans="3:5">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13"/>
     </row>
-    <row r="14" spans="3:5">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
@@ -2248,61 +2248,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBEBD98-CDDF-46A5-BB8F-EECC25228C81}">
   <dimension ref="C2:AU4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="12" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="12" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="34.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="34.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:47">
+    <row r="2" spans="3:47" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="3:47">
+    <row r="4" spans="3:47" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
@@ -2448,20 +2448,20 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="3:5">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="3:5">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2493,20 +2493,20 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="4" width="40.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="40.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="3:7">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>54</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2542,25 +2542,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353B38D8-CA51-4B54-B8E6-4750BDE5CEE1}">
   <dimension ref="B2:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D5" s="1"/>
     </row>
   </sheetData>
@@ -2586,15 +2586,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010025BF94C250D4F3428D6504CA93470C05" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0b958e8da78ae46a2ec6ca96c45141b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="05f9c4cf-3b22-4642-8b3f-b46f9e00fcab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b67ef449dd8e11e8882ef8210e0286c" ns2:_="">
     <xsd:import namespace="05f9c4cf-3b22-4642-8b3f-b46f9e00fcab"/>
@@ -2726,6 +2717,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2733,13 +2733,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8039B5D0-6D3B-4FB4-B652-0338149FBDAC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1F530B1-F3B4-4D56-BB52-37C0F4213D70}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="05f9c4cf-3b22-4642-8b3f-b46f9e00fcab"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1F530B1-F3B4-4D56-BB52-37C0F4213D70}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8039B5D0-6D3B-4FB4-B652-0338149FBDAC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E190EAA-270A-42C8-838D-8A23D09DF6DB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E190EAA-270A-42C8-838D-8A23D09DF6DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>